<commit_message>
UNIQUE,TRANSPOSE AND COUNTIF TEXT FNCTS,
</commit_message>
<xml_diff>
--- a/Formulas and Functions/8_Text_Functions.xlsx
+++ b/Formulas and Functions/8_Text_Functions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lee\Desktop\Excel\Excel_Data_Analytics_Project\Formulas and Functions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C5C8D04-CA72-4B19-8E98-C1CD6A64B189}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52EDA389-1645-4DAB-A014-84F9EB3E612F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="8" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -1484,16 +1484,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>588963</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>44450</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>106363</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>30163</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>117475</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>157163</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1786,8 +1786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B5E7F13-C613-4452-9CDB-2C26D6876D9D}">
   <dimension ref="A1:V21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1798,11 +1798,11 @@
     <col min="4" max="4" width="17.5546875" style="9" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="26.21875" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="11" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="32.33203125" customWidth="1"/>
-    <col min="8" max="8" width="3.5546875" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="8.88671875" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="0.21875" customWidth="1"/>
-    <col min="11" max="11" width="8.88671875" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="19.109375" customWidth="1"/>
+    <col min="8" max="8" width="37.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19" customWidth="1"/>
+    <col min="10" max="10" width="30.5546875" customWidth="1"/>
+    <col min="11" max="11" width="12.21875" customWidth="1"/>
     <col min="12" max="12" width="13.33203125" customWidth="1"/>
     <col min="13" max="13" width="15.44140625" customWidth="1"/>
     <col min="14" max="14" width="8.88671875" customWidth="1"/>
@@ -5555,8 +5555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85789AE4-586B-4DA1-B069-1172780CDADC}">
   <dimension ref="A2:BW25"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>